<commit_message>
agg sub items estado, contacts,clients. no terminado y en proceso
</commit_message>
<xml_diff>
--- a/doc/Vistas.xlsx
+++ b/doc/Vistas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\inmersal\admin_front\inmersal_admin_front\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\inmersal_front\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5853FAD-16C6-4874-BDE9-F793B62F81EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General_status" sheetId="8" r:id="rId1"/>
@@ -160,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,11 +504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -730,10 +729,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -856,7 +855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1006,11 +1005,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,16 +1122,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1486,11 +1486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se agg vista modal y se creo archivo exit.js en archivo layout, el item modal modal queda redirigido al archivo exit.js, se elimino archivo tablelist de logoutUser
</commit_message>
<xml_diff>
--- a/doc/Vistas.xlsx
+++ b/doc/Vistas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General_status" sheetId="8" r:id="rId1"/>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,12 +1268,13 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1489,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>